<commit_message>
Fixing CPU footprint on SMT board and updating bom + gerbers
</commit_message>
<xml_diff>
--- a/kicad-cpu-board-smt/bom/kicad-cpu-board-smt-all.xlsx
+++ b/kicad-cpu-board-smt/bom/kicad-cpu-board-smt-all.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="93">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">C13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-25.0000  2</t>
   </si>
   <si>
     <t xml:space="preserve">C14</t>
@@ -401,10 +398,10 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51:E51"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -412,7 +409,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,11 +724,11 @@
       <c r="D14" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>30</v>
+      <c r="E14" s="0" t="n">
+        <v>-25</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>70</v>
+        <v>270</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>10</v>
@@ -739,7 +736,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>8</v>
@@ -762,7 +759,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>21</v>
@@ -785,7 +782,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>21</v>
@@ -808,13 +805,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>42.4459</v>
@@ -831,13 +828,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>50.6781</v>
@@ -854,13 +851,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="C20" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>85.6005</v>
@@ -877,13 +874,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>80</v>
@@ -900,13 +897,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>58</v>
@@ -923,13 +920,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>71.6</v>
@@ -946,13 +943,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>64.8</v>
@@ -969,13 +966,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>17</v>
@@ -992,13 +989,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>24</v>
@@ -1015,13 +1012,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>31</v>
@@ -1038,13 +1035,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>38</v>
@@ -1061,13 +1058,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C29" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>53.8683</v>
@@ -1084,13 +1081,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="C30" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>56.576</v>
@@ -1107,13 +1104,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="C31" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>45.6895</v>
@@ -1130,13 +1127,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>48</v>
@@ -1153,13 +1150,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="C33" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>15.965</v>
@@ -1176,13 +1173,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>19.2607</v>
@@ -1199,13 +1196,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>22.5564</v>
@@ -1222,13 +1219,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>25.8521</v>
@@ -1245,13 +1242,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>29.1479</v>
@@ -1268,13 +1265,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>32.4436</v>
@@ -1291,13 +1288,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>35.7393</v>
@@ -1314,13 +1311,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>39.035</v>
@@ -1337,13 +1334,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>21</v>
@@ -1360,13 +1357,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>25</v>
@@ -1383,13 +1380,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>29</v>
@@ -1406,13 +1403,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>21</v>
@@ -1429,13 +1426,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>25</v>
@@ -1452,13 +1449,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>29</v>
@@ -1475,13 +1472,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="C47" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>64</v>
@@ -1498,13 +1495,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="C48" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>23</v>
@@ -1521,13 +1518,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="C49" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>46</v>
@@ -1544,13 +1541,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="C50" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>46</v>
@@ -1567,13 +1564,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="C51" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>18</v>
@@ -1590,13 +1587,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="C52" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>31</v>
@@ -1613,13 +1610,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>53.8226</v>
@@ -1636,7 +1633,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>